<commit_message>
Now generating a lattice graph for factors of production for each country.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/ChinaDataWorkbook.xlsx
+++ b/data/Excel Workbooks/ChinaDataWorkbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="285" windowWidth="15315" windowHeight="6030" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="280" windowWidth="18960" windowHeight="13300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="China Workbook" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,17 @@
     <sheet name="Employment calcs" sheetId="2" r:id="rId4"/>
     <sheet name="Exergy calcs" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
   <si>
     <t>Exergy [TJ]</t>
   </si>
@@ -849,6 +854,15 @@
   <si>
     <t>iX</t>
   </si>
+  <si>
+    <t>iU</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
 </sst>
 </file>
 
@@ -860,9 +874,9 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1140,6 +1154,22 @@
       <i/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1628,11 +1658,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1648,7 +1678,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -1657,12 +1687,12 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1671,7 +1701,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1680,7 +1710,7 @@
         <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1691,11 +1721,11 @@
         <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1704,7 +1734,7 @@
         <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
@@ -1713,7 +1743,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="463">
+  <cellStyleXfs count="467">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2183,6 +2213,10 @@
     <xf numFmtId="165" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2392,6 +2426,21 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2425,23 +2474,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="463">
+  <cellStyles count="467">
     <cellStyle name="•\Ž¦Ï‚Ý‚ÌƒnƒCƒp[ƒŠƒ“ƒN" xfId="42"/>
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 10" xfId="54"/>
@@ -2755,6 +2789,8 @@
     <cellStyle name="Explanatory Text 7" xfId="328"/>
     <cellStyle name="Explanatory Text 8" xfId="329"/>
     <cellStyle name="Explanatory Text 9" xfId="330"/>
+    <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
     <cellStyle name="ƒnƒCƒp[ƒŠƒ“ƒN" xfId="44"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Good 10" xfId="331"/>
@@ -2811,6 +2847,8 @@
     <cellStyle name="Heading 4 7" xfId="378"/>
     <cellStyle name="Heading 4 8" xfId="379"/>
     <cellStyle name="Heading 4 9" xfId="380"/>
+    <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Input 10" xfId="381"/>
     <cellStyle name="Input 11" xfId="382"/>
@@ -2937,10 +2975,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.9057244461108858E-2"/>
-          <c:y val="6.2731295876744975E-2"/>
-          <c:w val="0.88247631690877526"/>
-          <c:h val="0.80580865051545658"/>
+          <c:x val="0.0790572444611089"/>
+          <c:y val="0.062731295876745"/>
+          <c:w val="0.882476316908775"/>
+          <c:h val="0.805808650515457"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2971,67 +3009,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1991</c:v>
+                  <c:v>1991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1992</c:v>
+                  <c:v>1992.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1993</c:v>
+                  <c:v>1993.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1994</c:v>
+                  <c:v>1994.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1995</c:v>
+                  <c:v>1995.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1996</c:v>
+                  <c:v>1996.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1997</c:v>
+                  <c:v>1997.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1998</c:v>
+                  <c:v>1998.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1999</c:v>
+                  <c:v>1999.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2001</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2002</c:v>
+                  <c:v>2002.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2003</c:v>
+                  <c:v>2003.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2004</c:v>
+                  <c:v>2004.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2005</c:v>
+                  <c:v>2005.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2006</c:v>
+                  <c:v>2006.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2007</c:v>
+                  <c:v>2007.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2008</c:v>
+                  <c:v>2008.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2009</c:v>
+                  <c:v>2009.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2010</c:v>
+                  <c:v>2010.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2011</c:v>
+                  <c:v>2011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3043,67 +3081,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1420010626344625</c:v>
+                  <c:v>1.142001062634463</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3018805145938037</c:v>
+                  <c:v>1.301880514593804</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4724263777230009</c:v>
+                  <c:v>1.472426377723001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6329207640515988</c:v>
+                  <c:v>1.632920764051599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7962145824804676</c:v>
+                  <c:v>1.796214582480468</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9632624620021077</c:v>
+                  <c:v>1.963262462002108</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>2.116396798160423</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2772413312545186</c:v>
+                  <c:v>2.277241331254519</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4685312127098049</c:v>
+                  <c:v>2.468531212709805</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.6734193312370982</c:v>
+                  <c:v>2.673419331237098</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9166999102857791</c:v>
+                  <c:v>2.916699910285779</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2083704239214694</c:v>
+                  <c:v>3.208370423921469</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.5324147061641509</c:v>
+                  <c:v>3.532414706164151</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.9315785347838585</c:v>
+                  <c:v>3.931578534783859</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.4308878223832631</c:v>
+                  <c:v>4.430887822383263</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.0600736876028884</c:v>
+                  <c:v>5.060073687602888</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.5458422249126809</c:v>
+                  <c:v>5.54584222491268</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.056058322953775</c:v>
+                  <c:v>6.056058322953774</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.6844602775043764</c:v>
+                  <c:v>6.684460277504376</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3012882265327628</c:v>
+                  <c:v>7.301288226532763</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3135,67 +3173,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1991</c:v>
+                  <c:v>1991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1992</c:v>
+                  <c:v>1992.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1993</c:v>
+                  <c:v>1993.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1994</c:v>
+                  <c:v>1994.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1995</c:v>
+                  <c:v>1995.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1996</c:v>
+                  <c:v>1996.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1997</c:v>
+                  <c:v>1997.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1998</c:v>
+                  <c:v>1998.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1999</c:v>
+                  <c:v>1999.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2001</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2002</c:v>
+                  <c:v>2002.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2003</c:v>
+                  <c:v>2003.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2004</c:v>
+                  <c:v>2004.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2005</c:v>
+                  <c:v>2005.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2006</c:v>
+                  <c:v>2006.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2007</c:v>
+                  <c:v>2007.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2008</c:v>
+                  <c:v>2008.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2009</c:v>
+                  <c:v>2009.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2010</c:v>
+                  <c:v>2010.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2011</c:v>
+                  <c:v>2011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3207,67 +3245,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0985107132899505</c:v>
+                  <c:v>1.098510713289951</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2403796076615936</c:v>
+                  <c:v>1.240379607661594</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4015155899016787</c:v>
+                  <c:v>1.401515589901679</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5763081892356818</c:v>
+                  <c:v>1.576308189235682</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7664083693248671</c:v>
+                  <c:v>1.766408369324867</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9674541842240472</c:v>
+                  <c:v>1.967454184224047</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1905964336379244</c:v>
+                  <c:v>2.190596433637924</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2.422423120154733</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6766750310816048</c:v>
+                  <c:v>2.676675031081605</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2.951721368537525</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2685310368893497</c:v>
+                  <c:v>3.26853103688935</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.6488637897989209</c:v>
+                  <c:v>3.648863789798921</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.0734919941852414</c:v>
+                  <c:v>4.073491994185241</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>4.547123044576896</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.0819993231312024</c:v>
+                  <c:v>5.081999323131202</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.6910146543848299</c:v>
+                  <c:v>5.69101465438483</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3511651437118717</c:v>
+                  <c:v>6.351165143711871</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.2033298087056554</c:v>
+                  <c:v>7.203329808705655</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.1441590255894987</c:v>
+                  <c:v>8.144159025589498</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.189646888420107</c:v>
+                  <c:v>9.189646888420106</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3299,67 +3337,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1991</c:v>
+                  <c:v>1991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1992</c:v>
+                  <c:v>1992.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1993</c:v>
+                  <c:v>1993.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1994</c:v>
+                  <c:v>1994.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1995</c:v>
+                  <c:v>1995.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1996</c:v>
+                  <c:v>1996.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1997</c:v>
+                  <c:v>1997.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1998</c:v>
+                  <c:v>1998.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1999</c:v>
+                  <c:v>1999.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2001</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2002</c:v>
+                  <c:v>2002.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2003</c:v>
+                  <c:v>2003.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2004</c:v>
+                  <c:v>2004.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2005</c:v>
+                  <c:v>2005.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2006</c:v>
+                  <c:v>2006.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2007</c:v>
+                  <c:v>2007.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2008</c:v>
+                  <c:v>2008.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2009</c:v>
+                  <c:v>2009.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2010</c:v>
+                  <c:v>2010.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2011</c:v>
+                  <c:v>2011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3371,43 +3409,43 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.025828510517504</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0376896829396873</c:v>
+                  <c:v>1.037689682939687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0500601886449963</c:v>
+                  <c:v>1.050060188644996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0615313936827389</c:v>
+                  <c:v>1.061531393682739</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0727162591170047</c:v>
+                  <c:v>1.072716259117005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0837513469125288</c:v>
+                  <c:v>1.083751346912529</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0944003938069702</c:v>
+                  <c:v>1.09440039380697</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1039174170433839</c:v>
+                  <c:v>1.103917417043384</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1276859801371437</c:v>
+                  <c:v>1.127685980137144</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1205569990209538</c:v>
+                  <c:v>1.120556999020954</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1431311323141213</c:v>
+                  <c:v>1.143131132314121</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1654086471462513</c:v>
+                  <c:v>1.165408647146251</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1.15629138497367</c:v>
@@ -3416,10 +3454,10 @@
                   <c:v>1.17821720919724</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.2000044028108472</c:v>
+                  <c:v>1.200004402810847</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.2062880828655347</c:v>
+                  <c:v>1.206288082865535</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1.210779484188824</c:v>
@@ -3428,7 +3466,7 @@
                   <c:v>1.21692636170121</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.2381025261127236</c:v>
+                  <c:v>1.238102526112724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3460,67 +3498,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1991</c:v>
+                  <c:v>1991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1992</c:v>
+                  <c:v>1992.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1993</c:v>
+                  <c:v>1993.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1994</c:v>
+                  <c:v>1994.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1995</c:v>
+                  <c:v>1995.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1996</c:v>
+                  <c:v>1996.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1997</c:v>
+                  <c:v>1997.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1998</c:v>
+                  <c:v>1998.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1999</c:v>
+                  <c:v>1999.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2001</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2002</c:v>
+                  <c:v>2002.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2003</c:v>
+                  <c:v>2003.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2004</c:v>
+                  <c:v>2004.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2005</c:v>
+                  <c:v>2005.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2006</c:v>
+                  <c:v>2006.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2007</c:v>
+                  <c:v>2007.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2008</c:v>
+                  <c:v>2008.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2009</c:v>
+                  <c:v>2009.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2010</c:v>
+                  <c:v>2010.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2011</c:v>
+                  <c:v>2011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3532,64 +3570,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0366213248802143</c:v>
+                  <c:v>1.036621324880214</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1108781024150687</c:v>
+                  <c:v>1.110878102415069</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2024632189050535</c:v>
+                  <c:v>1.202463218905053</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2275638552830601</c:v>
+                  <c:v>1.22756385528306</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2564955425147335</c:v>
+                  <c:v>1.256495542514733</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.329778050327707</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3072971164374236</c:v>
+                  <c:v>1.307297116437424</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2872643612134995</c:v>
+                  <c:v>1.287264361213499</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2821747385970355</c:v>
+                  <c:v>1.282174738597035</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3521182332421211</c:v>
+                  <c:v>1.352118233242121</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5348872896516861</c:v>
+                  <c:v>1.534887289651686</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.7815265915004121</c:v>
+                  <c:v>1.781526591500412</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2.182969319144731</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3644818038645354</c:v>
+                  <c:v>2.364481803864535</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5214103933952701</c:v>
+                  <c:v>2.52141039339527</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6764382629405588</c:v>
+                  <c:v>2.676438262940559</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.9220325845937967</c:v>
+                  <c:v>2.922032584593797</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.1387065602417685</c:v>
+                  <c:v>3.138706560241769</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.6274136759601388</c:v>
+                  <c:v>3.627413675960139</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>3.977638557235311</c:v>
@@ -3628,67 +3666,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1991</c:v>
+                  <c:v>1991.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1992</c:v>
+                  <c:v>1992.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1993</c:v>
+                  <c:v>1993.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1994</c:v>
+                  <c:v>1994.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1995</c:v>
+                  <c:v>1995.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1996</c:v>
+                  <c:v>1996.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1997</c:v>
+                  <c:v>1997.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1998</c:v>
+                  <c:v>1998.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1999</c:v>
+                  <c:v>1999.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2000</c:v>
+                  <c:v>2000.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2001</c:v>
+                  <c:v>2001.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2002</c:v>
+                  <c:v>2002.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2003</c:v>
+                  <c:v>2003.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2004</c:v>
+                  <c:v>2004.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2005</c:v>
+                  <c:v>2005.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2006</c:v>
+                  <c:v>2006.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2007</c:v>
+                  <c:v>2007.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2008</c:v>
+                  <c:v>2008.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2009</c:v>
+                  <c:v>2009.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2010</c:v>
+                  <c:v>2010.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2011</c:v>
+                  <c:v>2011.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3700,67 +3738,67 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0356369180272185</c:v>
+                  <c:v>1.035636918027218</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1039265366559361</c:v>
+                  <c:v>1.103926536655936</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1877789207687233</c:v>
+                  <c:v>1.187778920768723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2122556580385555</c:v>
+                  <c:v>1.212255658038555</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2396467432711569</c:v>
+                  <c:v>1.239646743271157</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3058243542763346</c:v>
+                  <c:v>1.305824354276335</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2876704317734176</c:v>
+                  <c:v>1.287670431773418</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2715749612277882</c:v>
+                  <c:v>1.271574961227788</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.2702676832980084</c:v>
+                  <c:v>1.270267683298008</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3336253461802401</c:v>
+                  <c:v>1.33362534618024</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4992519748242048</c:v>
+                  <c:v>1.499251974824205</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.7220465820042674</c:v>
+                  <c:v>1.722046582004267</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.0814558466603676</c:v>
+                  <c:v>2.081455846660368</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.247094842642956</c:v>
+                  <c:v>2.247094842642955</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3910851407216209</c:v>
+                  <c:v>2.391085140721621</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.5309498330100566</c:v>
+                  <c:v>2.530949833010057</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>2.753317689867548</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.9488883061084867</c:v>
+                  <c:v>2.948888306108487</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.3926407069154623</c:v>
+                  <c:v>3.392640706915462</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.7110522855547847</c:v>
+                  <c:v>3.711052285554785</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3775,11 +3813,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="47522176"/>
-        <c:axId val="47524864"/>
+        <c:axId val="2090449480"/>
+        <c:axId val="2090457368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47522176"/>
+        <c:axId val="2090449480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3801,7 +3839,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3818,12 +3855,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47524864"/>
+        <c:crossAx val="2090457368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="47524864"/>
+        <c:axId val="2090457368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3845,7 +3882,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3862,7 +3898,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47522176"/>
+        <c:crossAx val="2090449480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3882,8 +3918,8 @@
     <sheetView zoomScale="98" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </chartsheet>
 </file>
 
@@ -4659,33 +4695,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC32"/>
   <sheetViews>
-    <sheetView topLeftCell="E4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" customWidth="1"/>
-    <col min="13" max="13" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="29.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" style="13" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.5" style="13" customWidth="1"/>
+    <col min="12" max="12" width="16.5" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:55" s="9" customFormat="1">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
       <c r="E1" s="83"/>
       <c r="G1" s="13"/>
       <c r="K1" s="13"/>
@@ -4958,35 +4994,35 @@
     </row>
     <row r="10" spans="1:55" ht="15" customHeight="1">
       <c r="A10" s="6"/>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="91" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="86" t="s">
+      <c r="E10" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="F10" s="86" t="s">
+      <c r="F10" s="91" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="84"/>
-      <c r="H10" s="86" t="s">
+      <c r="H10" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="86" t="s">
+      <c r="I10" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="86" t="s">
+      <c r="J10" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="86" t="s">
+      <c r="K10" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="L10" s="86" t="s">
+      <c r="L10" s="91" t="s">
         <v>41</v>
       </c>
     </row>
@@ -4994,38 +5030,38 @@
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="87"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="91"/>
+      <c r="D11" s="91"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="91"/>
       <c r="G11" s="84"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="L11" s="86"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="91"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="91"/>
+      <c r="L11" s="91"/>
     </row>
     <row r="12" spans="1:55">
       <c r="A12" s="12">
         <v>1991</v>
       </c>
-      <c r="B12" s="98">
+      <c r="B12" s="87">
         <v>574045</v>
       </c>
-      <c r="C12" s="97">
+      <c r="C12" s="86">
         <v>621421200</v>
       </c>
-      <c r="D12" s="98">
+      <c r="D12" s="87">
         <v>1140546</v>
       </c>
-      <c r="E12" s="98">
+      <c r="E12" s="87">
         <v>34884918.343168758</v>
       </c>
-      <c r="F12" s="97">
+      <c r="F12" s="86">
         <v>33799385.68615675</v>
       </c>
-      <c r="G12" s="96">
+      <c r="G12" s="85">
         <f>A12-$A$12</f>
         <v>0</v>
       </c>
@@ -5054,22 +5090,22 @@
       <c r="A13" s="12">
         <v>1992</v>
       </c>
-      <c r="B13" s="98">
+      <c r="B13" s="87">
         <v>655560</v>
       </c>
-      <c r="C13" s="97">
+      <c r="C13" s="86">
         <v>637471584</v>
       </c>
-      <c r="D13" s="98">
+      <c r="D13" s="87">
         <v>1252902</v>
       </c>
-      <c r="E13" s="98">
+      <c r="E13" s="87">
         <v>36128109.318550475</v>
       </c>
-      <c r="F13" s="97">
+      <c r="F13" s="86">
         <v>35037163.97012116</v>
       </c>
-      <c r="G13" s="96">
+      <c r="G13" s="85">
         <f t="shared" ref="G13:G32" si="1">A13-$A$12</f>
         <v>1</v>
       </c>
@@ -5098,22 +5134,22 @@
       <c r="A14" s="12">
         <v>1993</v>
       </c>
-      <c r="B14" s="98">
+      <c r="B14" s="87">
         <v>747338</v>
       </c>
-      <c r="C14" s="97">
+      <c r="C14" s="86">
         <v>644842368</v>
       </c>
-      <c r="D14" s="98">
+      <c r="D14" s="87">
         <v>1414710</v>
       </c>
-      <c r="E14" s="98">
+      <c r="E14" s="87">
         <v>38510387.08809942</v>
       </c>
-      <c r="F14" s="97">
+      <c r="F14" s="86">
         <v>37546997.433832847</v>
       </c>
-      <c r="G14" s="96">
+      <c r="G14" s="85">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -5142,22 +5178,22 @@
       <c r="A15" s="12">
         <v>1994</v>
       </c>
-      <c r="B15" s="98">
+      <c r="B15" s="87">
         <v>845239</v>
       </c>
-      <c r="C15" s="97">
+      <c r="C15" s="86">
         <v>652529662.5</v>
       </c>
-      <c r="D15" s="98">
+      <c r="D15" s="87">
         <v>1598493</v>
       </c>
-      <c r="E15" s="98">
+      <c r="E15" s="87">
         <v>41435570.660754025</v>
       </c>
-      <c r="F15" s="97">
+      <c r="F15" s="86">
         <v>40642518.109189436</v>
       </c>
-      <c r="G15" s="96">
+      <c r="G15" s="85">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -5186,22 +5222,22 @@
       <c r="A16" s="12">
         <v>1995</v>
       </c>
-      <c r="B16" s="98">
+      <c r="B16" s="87">
         <v>937370</v>
       </c>
-      <c r="C16" s="97">
+      <c r="C16" s="86">
         <v>659658112.5</v>
       </c>
-      <c r="D16" s="98">
+      <c r="D16" s="87">
         <v>1797852</v>
       </c>
-      <c r="E16" s="98">
+      <c r="E16" s="87">
         <v>42289439.641719319</v>
       </c>
-      <c r="F16" s="97">
+      <c r="F16" s="86">
         <v>41490904.199097656</v>
       </c>
-      <c r="G16" s="96">
+      <c r="G16" s="85">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -5230,22 +5266,22 @@
       <c r="A17" s="12">
         <v>1996</v>
       </c>
-      <c r="B17" s="98">
+      <c r="B17" s="87">
         <v>1031108</v>
       </c>
-      <c r="C17" s="97">
+      <c r="C17" s="86">
         <v>666608625</v>
       </c>
-      <c r="D17" s="98">
+      <c r="D17" s="87">
         <v>2014670</v>
       </c>
-      <c r="E17" s="98">
+      <c r="E17" s="87">
         <v>43244975.413389392</v>
       </c>
-      <c r="F17" s="97">
+      <c r="F17" s="86">
         <v>42468777.454392247</v>
       </c>
-      <c r="G17" s="96">
+      <c r="G17" s="85">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -5274,22 +5310,22 @@
       <c r="A18" s="12">
         <v>1997</v>
       </c>
-      <c r="B18" s="98">
+      <c r="B18" s="87">
         <v>1127001</v>
       </c>
-      <c r="C18" s="97">
+      <c r="C18" s="86">
         <v>673466062.5</v>
       </c>
-      <c r="D18" s="98">
+      <c r="D18" s="87">
         <v>2243972</v>
       </c>
-      <c r="E18" s="98">
+      <c r="E18" s="87">
         <v>45553575.969451003</v>
       </c>
-      <c r="F18" s="97">
+      <c r="F18" s="86">
         <v>44945681.20001173</v>
       </c>
-      <c r="G18" s="96">
+      <c r="G18" s="85">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -5318,22 +5354,22 @@
       <c r="A19" s="12">
         <v>1998</v>
       </c>
-      <c r="B19" s="98">
+      <c r="B19" s="87">
         <v>1214907</v>
       </c>
-      <c r="C19" s="97">
+      <c r="C19" s="86">
         <v>680083606</v>
       </c>
-      <c r="D19" s="98">
+      <c r="D19" s="87">
         <v>2498476</v>
       </c>
-      <c r="E19" s="98">
+      <c r="E19" s="87">
         <v>44920277.865328528</v>
       </c>
-      <c r="F19" s="97">
+      <c r="F19" s="86">
         <v>44185839.444869049</v>
       </c>
-      <c r="G19" s="96">
+      <c r="G19" s="85">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -5362,22 +5398,22 @@
       <c r="A20" s="12">
         <v>1999</v>
       </c>
-      <c r="B20" s="98">
+      <c r="B20" s="87">
         <v>1307239</v>
       </c>
-      <c r="C20" s="97">
+      <c r="C20" s="86">
         <v>685997686</v>
       </c>
-      <c r="D20" s="98">
+      <c r="D20" s="87">
         <v>2762885</v>
       </c>
-      <c r="E20" s="98">
+      <c r="E20" s="87">
         <v>44358788.689649373</v>
       </c>
-      <c r="F20" s="97">
+      <c r="F20" s="86">
         <v>43508744.624699265</v>
       </c>
-      <c r="G20" s="96">
+      <c r="G20" s="85">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -5406,22 +5442,22 @@
       <c r="A21" s="12">
         <v>2000</v>
       </c>
-      <c r="B21" s="98">
+      <c r="B21" s="87">
         <v>1417048</v>
       </c>
-      <c r="C21" s="97">
+      <c r="C21" s="86">
         <v>700767975</v>
       </c>
-      <c r="D21" s="98">
+      <c r="D21" s="87">
         <v>3052871</v>
       </c>
-      <c r="E21" s="98">
+      <c r="E21" s="87">
         <v>44313184.405817173</v>
       </c>
-      <c r="F21" s="97">
+      <c r="F21" s="86">
         <v>43336718.506888412</v>
       </c>
-      <c r="G21" s="96">
+      <c r="G21" s="85">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -5450,22 +5486,22 @@
       <c r="A22" s="12">
         <v>2001</v>
       </c>
-      <c r="B22" s="98">
+      <c r="B22" s="87">
         <v>1534663</v>
       </c>
-      <c r="C22" s="97">
+      <c r="C22" s="86">
         <v>696337875</v>
       </c>
-      <c r="D22" s="98">
+      <c r="D22" s="87">
         <v>3366574</v>
       </c>
-      <c r="E22" s="98">
+      <c r="E22" s="87">
         <v>46523411.301877841</v>
       </c>
-      <c r="F22" s="97">
+      <c r="F22" s="86">
         <v>45700765.658635303</v>
       </c>
-      <c r="G22" s="96">
+      <c r="G22" s="85">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -5494,22 +5530,22 @@
       <c r="A23" s="12">
         <v>2002</v>
       </c>
-      <c r="B23" s="98">
+      <c r="B23" s="87">
         <v>1674317</v>
       </c>
-      <c r="C23" s="97">
+      <c r="C23" s="86">
         <v>710365920</v>
       </c>
-      <c r="D23" s="98">
+      <c r="D23" s="87">
         <v>3727910</v>
       </c>
-      <c r="E23" s="98">
+      <c r="E23" s="87">
         <v>52301282.717576884</v>
       </c>
-      <c r="F23" s="97">
+      <c r="F23" s="86">
         <v>51878247.487717129</v>
       </c>
-      <c r="G23" s="96">
+      <c r="G23" s="85">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -5538,22 +5574,22 @@
       <c r="A24" s="12">
         <v>2003</v>
       </c>
-      <c r="B24" s="98">
+      <c r="B24" s="87">
         <v>1841749</v>
       </c>
-      <c r="C24" s="97">
+      <c r="C24" s="86">
         <v>724209640</v>
       </c>
-      <c r="D24" s="98">
+      <c r="D24" s="87">
         <v>4161697</v>
       </c>
-      <c r="E24" s="98">
+      <c r="E24" s="87">
         <v>60073454.396351732</v>
       </c>
-      <c r="F24" s="97">
+      <c r="F24" s="86">
         <v>60214504.376266651</v>
       </c>
-      <c r="G24" s="96">
+      <c r="G24" s="85">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -5582,22 +5618,22 @@
       <c r="A25" s="12">
         <v>2004</v>
       </c>
-      <c r="B25" s="98">
+      <c r="B25" s="87">
         <v>2027765</v>
       </c>
-      <c r="C25" s="97">
+      <c r="C25" s="86">
         <v>718543980</v>
       </c>
-      <c r="D25" s="98">
+      <c r="D25" s="87">
         <v>4646005</v>
       </c>
-      <c r="E25" s="98">
+      <c r="E25" s="87">
         <v>72611417.245658115</v>
       </c>
-      <c r="F25" s="97">
+      <c r="F25" s="86">
         <v>73783021.958819762</v>
       </c>
-      <c r="G25" s="96">
+      <c r="G25" s="85">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
@@ -5626,22 +5662,22 @@
       <c r="A26" s="12">
         <v>2005</v>
       </c>
-      <c r="B26" s="98">
+      <c r="B26" s="87">
         <v>2256903</v>
       </c>
-      <c r="C26" s="97">
+      <c r="C26" s="86">
         <v>732169152</v>
       </c>
-      <c r="D26" s="98">
+      <c r="D26" s="87">
         <v>5186203</v>
       </c>
-      <c r="E26" s="98">
+      <c r="E26" s="87">
         <v>78389720.094955176</v>
       </c>
-      <c r="F26" s="97">
+      <c r="F26" s="86">
         <v>79918032.436717063</v>
       </c>
-      <c r="G26" s="96">
+      <c r="G26" s="85">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
@@ -5670,22 +5706,22 @@
       <c r="A27" s="12">
         <v>2006</v>
       </c>
-      <c r="B27" s="98">
+      <c r="B27" s="87">
         <v>2543529</v>
       </c>
-      <c r="C27" s="97">
+      <c r="C27" s="86">
         <v>745708176</v>
       </c>
-      <c r="D27" s="98">
+      <c r="D27" s="87">
         <v>5796254</v>
       </c>
-      <c r="E27" s="98">
+      <c r="E27" s="87">
         <v>83412809.885637924</v>
       </c>
-      <c r="F27" s="97">
+      <c r="F27" s="86">
         <v>85222122.359450951</v>
       </c>
-      <c r="G27" s="96">
+      <c r="G27" s="85">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
@@ -5714,22 +5750,22 @@
       <c r="A28" s="12">
         <v>2007</v>
       </c>
-      <c r="B28" s="98">
+      <c r="B28" s="87">
         <v>2904710</v>
       </c>
-      <c r="C28" s="97">
+      <c r="C28" s="86">
         <v>749612988</v>
       </c>
-      <c r="D28" s="98">
+      <c r="D28" s="87">
         <v>6490864</v>
       </c>
-      <c r="E28" s="98">
+      <c r="E28" s="87">
         <v>88291978.255212426</v>
       </c>
-      <c r="F28" s="97">
+      <c r="F28" s="86">
         <v>90461969.114315361</v>
       </c>
-      <c r="G28" s="96">
+      <c r="G28" s="85">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
@@ -5758,22 +5794,22 @@
       <c r="A29" s="12">
         <v>2008</v>
       </c>
-      <c r="B29" s="98">
+      <c r="B29" s="87">
         <v>3183563</v>
       </c>
-      <c r="C29" s="97">
+      <c r="C29" s="86">
         <v>752404040</v>
       </c>
-      <c r="D29" s="98">
+      <c r="D29" s="87">
         <v>7243796</v>
       </c>
-      <c r="E29" s="98">
+      <c r="E29" s="87">
         <v>96049262.783831447</v>
       </c>
-      <c r="F29" s="97">
+      <c r="F29" s="86">
         <v>98762906.314203188</v>
       </c>
-      <c r="G29" s="96">
+      <c r="G29" s="85">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
@@ -5802,22 +5838,22 @@
       <c r="A30" s="12">
         <v>2009</v>
       </c>
-      <c r="B30" s="98">
+      <c r="B30" s="87">
         <v>3476450</v>
       </c>
-      <c r="C30" s="97">
+      <c r="C30" s="86">
         <v>756223840</v>
       </c>
-      <c r="D30" s="98">
+      <c r="D30" s="87">
         <v>8215729</v>
       </c>
-      <c r="E30" s="98">
+      <c r="E30" s="87">
         <v>102871727.76171979</v>
       </c>
-      <c r="F30" s="97">
+      <c r="F30" s="86">
         <v>106086353.58528192</v>
       </c>
-      <c r="G30" s="96">
+      <c r="G30" s="85">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
@@ -5846,22 +5882,22 @@
       <c r="A31" s="12">
         <v>2010</v>
       </c>
-      <c r="B31" s="98">
+      <c r="B31" s="87">
         <v>3837181</v>
       </c>
-      <c r="C31" s="97">
+      <c r="C31" s="86">
         <v>769383157.5</v>
       </c>
-      <c r="D31" s="98">
+      <c r="D31" s="87">
         <v>9288788</v>
       </c>
-      <c r="E31" s="98">
+      <c r="E31" s="87">
         <v>118351994.02845623</v>
       </c>
-      <c r="F31" s="97">
+      <c r="F31" s="86">
         <v>122604353.87701635</v>
       </c>
-      <c r="G31" s="96">
+      <c r="G31" s="85">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
@@ -5890,22 +5926,22 @@
       <c r="A32" s="12">
         <v>2011</v>
       </c>
-      <c r="B32" s="98">
+      <c r="B32" s="87">
         <v>4191268</v>
       </c>
-      <c r="C32" s="98" t="s">
+      <c r="C32" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="98">
+      <c r="D32" s="87">
         <v>10481215</v>
       </c>
-      <c r="E32" s="98">
+      <c r="E32" s="87">
         <v>129459755.94880845</v>
       </c>
-      <c r="F32" s="97">
+      <c r="F32" s="86">
         <v>134441739.71612436</v>
       </c>
-      <c r="G32" s="96">
+      <c r="G32" s="85">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -5944,593 +5980,826 @@
     <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection sqref="A1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="9" width="8.83203125" style="26"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="98" t="str">
+    <row r="1" spans="1:9">
+      <c r="A1" s="26" t="str">
+        <f>'China Workbook'!A11</f>
+        <v>Year</v>
+      </c>
+      <c r="B1" s="87" t="str">
         <f>'China Workbook'!G9</f>
         <v>iYear</v>
       </c>
-      <c r="B1" s="98" t="str">
+      <c r="C1" s="87" t="str">
         <f>'China Workbook'!H9</f>
         <v>iGDP</v>
       </c>
-      <c r="C1" s="98" t="str">
+      <c r="D1" s="87" t="str">
         <f>'China Workbook'!I9</f>
         <v>iLabor</v>
       </c>
-      <c r="D1" s="98" t="str">
+      <c r="E1" s="87" t="str">
         <f>'China Workbook'!J9</f>
         <v>iCapStk</v>
       </c>
-      <c r="E1" s="98" t="str">
+      <c r="F1" s="87" t="str">
         <f>'China Workbook'!K9</f>
         <v>iQ</v>
       </c>
-      <c r="F1" s="98" t="str">
+      <c r="G1" s="87" t="str">
         <f>'China Workbook'!L9</f>
         <v>iX</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="99">
+      <c r="H1" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="26">
+        <f>'China Workbook'!A12</f>
+        <v>1991</v>
+      </c>
+      <c r="B2" s="88">
         <f>'China Workbook'!G12</f>
         <v>0</v>
       </c>
-      <c r="B2" s="100">
+      <c r="C2" s="89">
         <f>'China Workbook'!H12</f>
         <v>1</v>
       </c>
-      <c r="C2" s="100">
+      <c r="D2" s="89">
         <f>'China Workbook'!I12</f>
         <v>1</v>
       </c>
-      <c r="D2" s="100">
+      <c r="E2" s="89">
         <f>'China Workbook'!J12</f>
         <v>1</v>
       </c>
-      <c r="E2" s="100">
+      <c r="F2" s="89">
         <f>'China Workbook'!K12</f>
         <v>1</v>
       </c>
-      <c r="F2" s="100">
+      <c r="G2" s="89">
         <f>'China Workbook'!L12</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="99">
+      <c r="H2" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="26">
+        <f>'China Workbook'!A13</f>
+        <v>1992</v>
+      </c>
+      <c r="B3" s="88">
         <f>'China Workbook'!G13</f>
         <v>1</v>
       </c>
-      <c r="B3" s="100">
+      <c r="C3" s="89">
         <f>'China Workbook'!H13</f>
         <v>1.1420010626344625</v>
       </c>
-      <c r="C3" s="100">
+      <c r="D3" s="89">
         <f>'China Workbook'!I13</f>
         <v>1.025828510517504</v>
       </c>
-      <c r="D3" s="100">
+      <c r="E3" s="89">
         <f>'China Workbook'!J13</f>
         <v>1.0985107132899505</v>
       </c>
-      <c r="E3" s="100">
+      <c r="F3" s="89">
         <f>'China Workbook'!K13</f>
         <v>1.0356369180272185</v>
       </c>
-      <c r="F3" s="100">
+      <c r="G3" s="89">
         <f>'China Workbook'!L13</f>
         <v>1.0366213248802143</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="99">
+      <c r="H3" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="26">
+        <f>'China Workbook'!A14</f>
+        <v>1993</v>
+      </c>
+      <c r="B4" s="88">
         <f>'China Workbook'!G14</f>
         <v>2</v>
       </c>
-      <c r="B4" s="100">
+      <c r="C4" s="89">
         <f>'China Workbook'!H14</f>
         <v>1.3018805145938037</v>
       </c>
-      <c r="C4" s="100">
+      <c r="D4" s="89">
         <f>'China Workbook'!I14</f>
         <v>1.0376896829396873</v>
       </c>
-      <c r="D4" s="100">
+      <c r="E4" s="89">
         <f>'China Workbook'!J14</f>
         <v>1.2403796076615936</v>
       </c>
-      <c r="E4" s="100">
+      <c r="F4" s="89">
         <f>'China Workbook'!K14</f>
         <v>1.1039265366559361</v>
       </c>
-      <c r="F4" s="100">
+      <c r="G4" s="89">
         <f>'China Workbook'!L14</f>
         <v>1.1108781024150687</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="99">
+      <c r="H4" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I4" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="26">
+        <f>'China Workbook'!A15</f>
+        <v>1994</v>
+      </c>
+      <c r="B5" s="88">
         <f>'China Workbook'!G15</f>
         <v>3</v>
       </c>
-      <c r="B5" s="100">
+      <c r="C5" s="89">
         <f>'China Workbook'!H15</f>
         <v>1.4724263777230009</v>
       </c>
-      <c r="C5" s="100">
+      <c r="D5" s="89">
         <f>'China Workbook'!I15</f>
         <v>1.0500601886449963</v>
       </c>
-      <c r="D5" s="100">
+      <c r="E5" s="89">
         <f>'China Workbook'!J15</f>
         <v>1.4015155899016787</v>
       </c>
-      <c r="E5" s="100">
+      <c r="F5" s="89">
         <f>'China Workbook'!K15</f>
         <v>1.1877789207687233</v>
       </c>
-      <c r="F5" s="100">
+      <c r="G5" s="89">
         <f>'China Workbook'!L15</f>
         <v>1.2024632189050535</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="99">
+      <c r="H5" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I5" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="26">
+        <f>'China Workbook'!A16</f>
+        <v>1995</v>
+      </c>
+      <c r="B6" s="88">
         <f>'China Workbook'!G16</f>
         <v>4</v>
       </c>
-      <c r="B6" s="100">
+      <c r="C6" s="89">
         <f>'China Workbook'!H16</f>
         <v>1.6329207640515988</v>
       </c>
-      <c r="C6" s="100">
+      <c r="D6" s="89">
         <f>'China Workbook'!I16</f>
         <v>1.0615313936827389</v>
       </c>
-      <c r="D6" s="100">
+      <c r="E6" s="89">
         <f>'China Workbook'!J16</f>
         <v>1.5763081892356818</v>
       </c>
-      <c r="E6" s="100">
+      <c r="F6" s="89">
         <f>'China Workbook'!K16</f>
         <v>1.2122556580385555</v>
       </c>
-      <c r="F6" s="100">
+      <c r="G6" s="89">
         <f>'China Workbook'!L16</f>
         <v>1.2275638552830601</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="99">
+      <c r="H6" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="26">
+        <f>'China Workbook'!A17</f>
+        <v>1996</v>
+      </c>
+      <c r="B7" s="88">
         <f>'China Workbook'!G17</f>
         <v>5</v>
       </c>
-      <c r="B7" s="100">
+      <c r="C7" s="89">
         <f>'China Workbook'!H17</f>
         <v>1.7962145824804676</v>
       </c>
-      <c r="C7" s="100">
+      <c r="D7" s="89">
         <f>'China Workbook'!I17</f>
         <v>1.0727162591170047</v>
       </c>
-      <c r="D7" s="100">
+      <c r="E7" s="89">
         <f>'China Workbook'!J17</f>
         <v>1.7664083693248671</v>
       </c>
-      <c r="E7" s="100">
+      <c r="F7" s="89">
         <f>'China Workbook'!K17</f>
         <v>1.2396467432711569</v>
       </c>
-      <c r="F7" s="100">
+      <c r="G7" s="89">
         <f>'China Workbook'!L17</f>
         <v>1.2564955425147335</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="99">
+      <c r="H7" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="26">
+        <f>'China Workbook'!A18</f>
+        <v>1997</v>
+      </c>
+      <c r="B8" s="88">
         <f>'China Workbook'!G18</f>
         <v>6</v>
       </c>
-      <c r="B8" s="100">
+      <c r="C8" s="89">
         <f>'China Workbook'!H18</f>
         <v>1.9632624620021077</v>
       </c>
-      <c r="C8" s="100">
+      <c r="D8" s="89">
         <f>'China Workbook'!I18</f>
         <v>1.0837513469125288</v>
       </c>
-      <c r="D8" s="100">
+      <c r="E8" s="89">
         <f>'China Workbook'!J18</f>
         <v>1.9674541842240472</v>
       </c>
-      <c r="E8" s="100">
+      <c r="F8" s="89">
         <f>'China Workbook'!K18</f>
         <v>1.3058243542763346</v>
       </c>
-      <c r="F8" s="100">
+      <c r="G8" s="89">
         <f>'China Workbook'!L18</f>
         <v>1.329778050327707</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="99">
+      <c r="H8" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="26">
+        <f>'China Workbook'!A19</f>
+        <v>1998</v>
+      </c>
+      <c r="B9" s="88">
         <f>'China Workbook'!G19</f>
         <v>7</v>
       </c>
-      <c r="B9" s="100">
+      <c r="C9" s="89">
         <f>'China Workbook'!H19</f>
         <v>2.116396798160423</v>
       </c>
-      <c r="C9" s="100">
+      <c r="D9" s="89">
         <f>'China Workbook'!I19</f>
         <v>1.0944003938069702</v>
       </c>
-      <c r="D9" s="100">
+      <c r="E9" s="89">
         <f>'China Workbook'!J19</f>
         <v>2.1905964336379244</v>
       </c>
-      <c r="E9" s="100">
+      <c r="F9" s="89">
         <f>'China Workbook'!K19</f>
         <v>1.2876704317734176</v>
       </c>
-      <c r="F9" s="100">
+      <c r="G9" s="89">
         <f>'China Workbook'!L19</f>
         <v>1.3072971164374236</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="99">
+      <c r="H9" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="26">
+        <f>'China Workbook'!A20</f>
+        <v>1999</v>
+      </c>
+      <c r="B10" s="88">
         <f>'China Workbook'!G20</f>
         <v>8</v>
       </c>
-      <c r="B10" s="100">
+      <c r="C10" s="89">
         <f>'China Workbook'!H20</f>
         <v>2.2772413312545186</v>
       </c>
-      <c r="C10" s="100">
+      <c r="D10" s="89">
         <f>'China Workbook'!I20</f>
         <v>1.1039174170433839</v>
       </c>
-      <c r="D10" s="100">
+      <c r="E10" s="89">
         <f>'China Workbook'!J20</f>
         <v>2.422423120154733</v>
       </c>
-      <c r="E10" s="100">
+      <c r="F10" s="89">
         <f>'China Workbook'!K20</f>
         <v>1.2715749612277882</v>
       </c>
-      <c r="F10" s="100">
+      <c r="G10" s="89">
         <f>'China Workbook'!L20</f>
         <v>1.2872643612134995</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="99">
+      <c r="H10" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="26">
+        <f>'China Workbook'!A21</f>
+        <v>2000</v>
+      </c>
+      <c r="B11" s="88">
         <f>'China Workbook'!G21</f>
         <v>9</v>
       </c>
-      <c r="B11" s="100">
+      <c r="C11" s="89">
         <f>'China Workbook'!H21</f>
         <v>2.4685312127098049</v>
       </c>
-      <c r="C11" s="100">
+      <c r="D11" s="89">
         <f>'China Workbook'!I21</f>
         <v>1.1276859801371437</v>
       </c>
-      <c r="D11" s="100">
+      <c r="E11" s="89">
         <f>'China Workbook'!J21</f>
         <v>2.6766750310816048</v>
       </c>
-      <c r="E11" s="100">
+      <c r="F11" s="89">
         <f>'China Workbook'!K21</f>
         <v>1.2702676832980084</v>
       </c>
-      <c r="F11" s="100">
+      <c r="G11" s="89">
         <f>'China Workbook'!L21</f>
         <v>1.2821747385970355</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="99">
+      <c r="H11" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="26">
+        <f>'China Workbook'!A22</f>
+        <v>2001</v>
+      </c>
+      <c r="B12" s="88">
         <f>'China Workbook'!G22</f>
         <v>10</v>
       </c>
-      <c r="B12" s="100">
+      <c r="C12" s="89">
         <f>'China Workbook'!H22</f>
         <v>2.6734193312370982</v>
       </c>
-      <c r="C12" s="100">
+      <c r="D12" s="89">
         <f>'China Workbook'!I22</f>
         <v>1.1205569990209538</v>
       </c>
-      <c r="D12" s="100">
+      <c r="E12" s="89">
         <f>'China Workbook'!J22</f>
         <v>2.951721368537525</v>
       </c>
-      <c r="E12" s="100">
+      <c r="F12" s="89">
         <f>'China Workbook'!K22</f>
         <v>1.3336253461802401</v>
       </c>
-      <c r="F12" s="100">
+      <c r="G12" s="89">
         <f>'China Workbook'!L22</f>
         <v>1.3521182332421211</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="99">
+      <c r="H12" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="26">
+        <f>'China Workbook'!A23</f>
+        <v>2002</v>
+      </c>
+      <c r="B13" s="88">
         <f>'China Workbook'!G23</f>
         <v>11</v>
       </c>
-      <c r="B13" s="100">
+      <c r="C13" s="89">
         <f>'China Workbook'!H23</f>
         <v>2.9166999102857791</v>
       </c>
-      <c r="C13" s="100">
+      <c r="D13" s="89">
         <f>'China Workbook'!I23</f>
         <v>1.1431311323141213</v>
       </c>
-      <c r="D13" s="100">
+      <c r="E13" s="89">
         <f>'China Workbook'!J23</f>
         <v>3.2685310368893497</v>
       </c>
-      <c r="E13" s="100">
+      <c r="F13" s="89">
         <f>'China Workbook'!K23</f>
         <v>1.4992519748242048</v>
       </c>
-      <c r="F13" s="100">
+      <c r="G13" s="89">
         <f>'China Workbook'!L23</f>
         <v>1.5348872896516861</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="99">
+      <c r="H13" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="26">
+        <f>'China Workbook'!A24</f>
+        <v>2003</v>
+      </c>
+      <c r="B14" s="88">
         <f>'China Workbook'!G24</f>
         <v>12</v>
       </c>
-      <c r="B14" s="100">
+      <c r="C14" s="89">
         <f>'China Workbook'!H24</f>
         <v>3.2083704239214694</v>
       </c>
-      <c r="C14" s="100">
+      <c r="D14" s="89">
         <f>'China Workbook'!I24</f>
         <v>1.1654086471462513</v>
       </c>
-      <c r="D14" s="100">
+      <c r="E14" s="89">
         <f>'China Workbook'!J24</f>
         <v>3.6488637897989209</v>
       </c>
-      <c r="E14" s="100">
+      <c r="F14" s="89">
         <f>'China Workbook'!K24</f>
         <v>1.7220465820042674</v>
       </c>
-      <c r="F14" s="100">
+      <c r="G14" s="89">
         <f>'China Workbook'!L24</f>
         <v>1.7815265915004121</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="99">
+      <c r="H14" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="26">
+        <f>'China Workbook'!A25</f>
+        <v>2004</v>
+      </c>
+      <c r="B15" s="88">
         <f>'China Workbook'!G25</f>
         <v>13</v>
       </c>
-      <c r="B15" s="100">
+      <c r="C15" s="89">
         <f>'China Workbook'!H25</f>
         <v>3.5324147061641509</v>
       </c>
-      <c r="C15" s="100">
+      <c r="D15" s="89">
         <f>'China Workbook'!I25</f>
         <v>1.15629138497367</v>
       </c>
-      <c r="D15" s="100">
+      <c r="E15" s="89">
         <f>'China Workbook'!J25</f>
         <v>4.0734919941852414</v>
       </c>
-      <c r="E15" s="100">
+      <c r="F15" s="89">
         <f>'China Workbook'!K25</f>
         <v>2.0814558466603676</v>
       </c>
-      <c r="F15" s="100">
+      <c r="G15" s="89">
         <f>'China Workbook'!L25</f>
         <v>2.182969319144731</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="99">
+      <c r="H15" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I15" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="26">
+        <f>'China Workbook'!A26</f>
+        <v>2005</v>
+      </c>
+      <c r="B16" s="88">
         <f>'China Workbook'!G26</f>
         <v>14</v>
       </c>
-      <c r="B16" s="100">
+      <c r="C16" s="89">
         <f>'China Workbook'!H26</f>
         <v>3.9315785347838585</v>
       </c>
-      <c r="C16" s="100">
+      <c r="D16" s="89">
         <f>'China Workbook'!I26</f>
         <v>1.17821720919724</v>
       </c>
-      <c r="D16" s="100">
+      <c r="E16" s="89">
         <f>'China Workbook'!J26</f>
         <v>4.547123044576896</v>
       </c>
-      <c r="E16" s="100">
+      <c r="F16" s="89">
         <f>'China Workbook'!K26</f>
         <v>2.247094842642956</v>
       </c>
-      <c r="F16" s="100">
+      <c r="G16" s="89">
         <f>'China Workbook'!L26</f>
         <v>2.3644818038645354</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="99">
+      <c r="H16" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I16" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="26">
+        <f>'China Workbook'!A27</f>
+        <v>2006</v>
+      </c>
+      <c r="B17" s="88">
         <f>'China Workbook'!G27</f>
         <v>15</v>
       </c>
-      <c r="B17" s="100">
+      <c r="C17" s="89">
         <f>'China Workbook'!H27</f>
         <v>4.4308878223832631</v>
       </c>
-      <c r="C17" s="100">
+      <c r="D17" s="89">
         <f>'China Workbook'!I27</f>
         <v>1.2000044028108472</v>
       </c>
-      <c r="D17" s="100">
+      <c r="E17" s="89">
         <f>'China Workbook'!J27</f>
         <v>5.0819993231312024</v>
       </c>
-      <c r="E17" s="100">
+      <c r="F17" s="89">
         <f>'China Workbook'!K27</f>
         <v>2.3910851407216209</v>
       </c>
-      <c r="F17" s="100">
+      <c r="G17" s="89">
         <f>'China Workbook'!L27</f>
         <v>2.5214103933952701</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="99">
+      <c r="H17" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I17" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="26">
+        <f>'China Workbook'!A28</f>
+        <v>2007</v>
+      </c>
+      <c r="B18" s="88">
         <f>'China Workbook'!G28</f>
         <v>16</v>
       </c>
-      <c r="B18" s="100">
+      <c r="C18" s="89">
         <f>'China Workbook'!H28</f>
         <v>5.0600736876028884</v>
       </c>
-      <c r="C18" s="100">
+      <c r="D18" s="89">
         <f>'China Workbook'!I28</f>
         <v>1.2062880828655347</v>
       </c>
-      <c r="D18" s="100">
+      <c r="E18" s="89">
         <f>'China Workbook'!J28</f>
         <v>5.6910146543848299</v>
       </c>
-      <c r="E18" s="100">
+      <c r="F18" s="89">
         <f>'China Workbook'!K28</f>
         <v>2.5309498330100566</v>
       </c>
-      <c r="F18" s="100">
+      <c r="G18" s="89">
         <f>'China Workbook'!L28</f>
         <v>2.6764382629405588</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="99">
+      <c r="H18" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="26">
+        <f>'China Workbook'!A29</f>
+        <v>2008</v>
+      </c>
+      <c r="B19" s="88">
         <f>'China Workbook'!G29</f>
         <v>17</v>
       </c>
-      <c r="B19" s="100">
+      <c r="C19" s="89">
         <f>'China Workbook'!H29</f>
         <v>5.5458422249126809</v>
       </c>
-      <c r="C19" s="100">
+      <c r="D19" s="89">
         <f>'China Workbook'!I29</f>
         <v>1.210779484188824</v>
       </c>
-      <c r="D19" s="100">
+      <c r="E19" s="89">
         <f>'China Workbook'!J29</f>
         <v>6.3511651437118717</v>
       </c>
-      <c r="E19" s="100">
+      <c r="F19" s="89">
         <f>'China Workbook'!K29</f>
         <v>2.753317689867548</v>
       </c>
-      <c r="F19" s="100">
+      <c r="G19" s="89">
         <f>'China Workbook'!L29</f>
         <v>2.9220325845937967</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="99">
+      <c r="H19" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="26">
+        <f>'China Workbook'!A30</f>
+        <v>2009</v>
+      </c>
+      <c r="B20" s="88">
         <f>'China Workbook'!G30</f>
         <v>18</v>
       </c>
-      <c r="B20" s="100">
+      <c r="C20" s="89">
         <f>'China Workbook'!H30</f>
         <v>6.056058322953775</v>
       </c>
-      <c r="C20" s="100">
+      <c r="D20" s="89">
         <f>'China Workbook'!I30</f>
         <v>1.21692636170121</v>
       </c>
-      <c r="D20" s="100">
+      <c r="E20" s="89">
         <f>'China Workbook'!J30</f>
         <v>7.2033298087056554</v>
       </c>
-      <c r="E20" s="100">
+      <c r="F20" s="89">
         <f>'China Workbook'!K30</f>
         <v>2.9488883061084867</v>
       </c>
-      <c r="F20" s="100">
+      <c r="G20" s="89">
         <f>'China Workbook'!L30</f>
         <v>3.1387065602417685</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="99">
+      <c r="H20" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="26">
+        <f>'China Workbook'!A31</f>
+        <v>2010</v>
+      </c>
+      <c r="B21" s="88">
         <f>'China Workbook'!G31</f>
         <v>19</v>
       </c>
-      <c r="B21" s="100">
+      <c r="C21" s="89">
         <f>'China Workbook'!H31</f>
         <v>6.6844602775043764</v>
       </c>
-      <c r="C21" s="100">
+      <c r="D21" s="89">
         <f>'China Workbook'!I31</f>
         <v>1.2381025261127236</v>
       </c>
-      <c r="D21" s="100">
+      <c r="E21" s="89">
         <f>'China Workbook'!J31</f>
         <v>8.1441590255894987</v>
       </c>
-      <c r="E21" s="100">
+      <c r="F21" s="89">
         <f>'China Workbook'!K31</f>
         <v>3.3926407069154623</v>
       </c>
-      <c r="F21" s="100">
+      <c r="G21" s="89">
         <f>'China Workbook'!L31</f>
         <v>3.6274136759601388</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="99">
+      <c r="H21" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="26">
+        <f>'China Workbook'!A32</f>
+        <v>2011</v>
+      </c>
+      <c r="B22" s="88">
         <f>'China Workbook'!G32</f>
         <v>20</v>
       </c>
-      <c r="B22" s="100">
+      <c r="C22" s="89">
         <f>'China Workbook'!H32</f>
         <v>7.3012882265327628</v>
       </c>
-      <c r="C22" s="100" t="str">
+      <c r="D22" s="89" t="str">
         <f>'China Workbook'!I32</f>
         <v>NA</v>
       </c>
-      <c r="D22" s="100">
+      <c r="E22" s="89">
         <f>'China Workbook'!J32</f>
         <v>9.189646888420107</v>
       </c>
-      <c r="E22" s="100">
+      <c r="F22" s="89">
         <f>'China Workbook'!K32</f>
         <v>3.7110522855547847</v>
       </c>
-      <c r="F22" s="100">
+      <c r="G22" s="89">
         <f>'China Workbook'!L32</f>
         <v>3.977638557235311</v>
       </c>
+      <c r="H22" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6542,20 +6811,20 @@
       <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.83203125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="13" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="13" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.5" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54">
@@ -6743,34 +7012,34 @@
     </row>
     <row r="7" spans="1:54" ht="15" customHeight="1">
       <c r="A7" s="4"/>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="85" t="s">
+      <c r="C7" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="85" t="s">
+      <c r="E7" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="85" t="s">
+      <c r="F7" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="85" t="s">
+      <c r="G7" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="85" t="s">
+      <c r="H7" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="85" t="s">
+      <c r="I7" s="90" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="85" t="s">
+      <c r="J7" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="K7" s="85" t="s">
+      <c r="K7" s="90" t="s">
         <v>45</v>
       </c>
     </row>
@@ -6778,16 +7047,16 @@
       <c r="A8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="90"/>
+      <c r="F8" s="90"/>
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
     </row>
     <row r="9" spans="1:54">
       <c r="A9" s="4">
@@ -7484,6 +7753,11 @@
     <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -7495,42 +7769,42 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="13" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" style="13" customWidth="1"/>
     <col min="4" max="4" width="48" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" style="13" customWidth="1"/>
-    <col min="6" max="6" width="40.5703125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" style="13" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="13" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="13" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" style="13" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.28515625" style="13" customWidth="1"/>
-    <col min="23" max="23" width="14.28515625" style="13" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.7109375" style="13" customWidth="1"/>
-    <col min="26" max="26" width="19.7109375" style="13" customWidth="1"/>
-    <col min="27" max="27" width="18.85546875" style="13" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="40.5" style="13" customWidth="1"/>
+    <col min="7" max="7" width="23.5" style="13" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="17.83203125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="24.5" style="13" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.1640625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="26.6640625" style="13" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="13" customWidth="1"/>
+    <col min="16" max="16" width="17.83203125" style="13" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" style="13" customWidth="1"/>
+    <col min="23" max="23" width="14.33203125" style="13" customWidth="1"/>
+    <col min="24" max="24" width="15.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" style="13" customWidth="1"/>
+    <col min="26" max="26" width="19.6640625" style="13" customWidth="1"/>
+    <col min="27" max="27" width="18.83203125" style="13" customWidth="1"/>
+    <col min="28" max="28" width="19.5" style="13" customWidth="1"/>
     <col min="29" max="29" width="17" style="13" customWidth="1"/>
-    <col min="30" max="30" width="14.85546875" style="13" customWidth="1"/>
-    <col min="31" max="31" width="20.7109375" style="13" customWidth="1"/>
-    <col min="32" max="32" width="24.42578125" style="13" customWidth="1"/>
-    <col min="33" max="33" width="15.140625" style="13" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="13"/>
+    <col min="30" max="30" width="14.83203125" style="13" customWidth="1"/>
+    <col min="31" max="31" width="20.6640625" style="13" customWidth="1"/>
+    <col min="32" max="32" width="24.5" style="13" customWidth="1"/>
+    <col min="33" max="33" width="15.1640625" style="13" customWidth="1"/>
+    <col min="34" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -7601,7 +7875,7 @@
     <row r="14" spans="1:7">
       <c r="A14" s="34"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1">
+    <row r="15" spans="1:7" ht="15" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -7612,7 +7886,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18">
+    <row r="16" spans="1:7" ht="16">
       <c r="A16" s="35" t="s">
         <v>13</v>
       </c>
@@ -7635,7 +7909,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="18">
+    <row r="17" spans="1:33" ht="16">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -7682,7 +7956,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="18">
+    <row r="19" spans="1:33" ht="16">
       <c r="A19" s="16" t="s">
         <v>20</v>
       </c>
@@ -7703,7 +7977,7 @@
       </c>
       <c r="G19" s="40"/>
     </row>
-    <row r="20" spans="1:33" ht="19.5" thickBot="1">
+    <row r="20" spans="1:33" ht="18" thickBot="1">
       <c r="A20" s="42" t="s">
         <v>54</v>
       </c>
@@ -7724,7 +7998,7 @@
       </c>
       <c r="G20" s="40"/>
     </row>
-    <row r="21" spans="1:33" ht="18.75">
+    <row r="21" spans="1:33" ht="17">
       <c r="A21" s="45"/>
       <c r="B21" s="46"/>
       <c r="C21" s="47">
@@ -7741,7 +8015,7 @@
       </c>
       <c r="G21" s="40"/>
     </row>
-    <row r="22" spans="1:33" ht="18">
+    <row r="22" spans="1:33" ht="16">
       <c r="A22" s="27"/>
       <c r="B22" s="27"/>
       <c r="C22" s="44">
@@ -7759,7 +8033,7 @@
       </c>
       <c r="G22" s="40"/>
     </row>
-    <row r="23" spans="1:33" ht="15.75" thickBot="1">
+    <row r="23" spans="1:33" ht="15" thickBot="1">
       <c r="A23" s="28"/>
       <c r="B23" s="29"/>
       <c r="C23" s="39">
@@ -7778,7 +8052,7 @@
       </c>
       <c r="G23" s="81"/>
     </row>
-    <row r="24" spans="1:33" ht="18" thickBot="1">
+    <row r="24" spans="1:33" ht="17" thickBot="1">
       <c r="A24" s="48"/>
       <c r="C24" s="49">
         <f>1000/6</f>
@@ -7796,7 +8070,7 @@
       <c r="A26" s="48"/>
       <c r="C26" s="51"/>
     </row>
-    <row r="27" spans="1:33" ht="15.75" thickBot="1">
+    <row r="27" spans="1:33" ht="15" thickBot="1">
       <c r="E27" s="26" t="s">
         <v>58</v>
       </c>
@@ -7811,140 +8085,140 @@
       </c>
     </row>
     <row r="28" spans="1:33" ht="15" customHeight="1">
-      <c r="A28" s="92" t="s">
+      <c r="A28" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="88" t="s">
+      <c r="B28" s="93" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="94" t="s">
+      <c r="C28" s="99" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="88" t="s">
+      <c r="D28" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="88" t="s">
+      <c r="E28" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="88" t="s">
+      <c r="F28" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="88" t="s">
+      <c r="G28" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="88" t="s">
+      <c r="H28" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="I28" s="88" t="s">
+      <c r="I28" s="93" t="s">
         <v>68</v>
       </c>
-      <c r="J28" s="88" t="s">
+      <c r="J28" s="93" t="s">
         <v>75</v>
       </c>
-      <c r="K28" s="88" t="s">
+      <c r="K28" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="L28" s="92" t="s">
+      <c r="L28" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="M28" s="94" t="s">
+      <c r="M28" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="N28" s="88" t="s">
+      <c r="N28" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="O28" s="88" t="s">
+      <c r="O28" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="P28" s="92" t="s">
+      <c r="P28" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="Q28" s="94" t="s">
+      <c r="Q28" s="99" t="s">
         <v>28</v>
       </c>
-      <c r="R28" s="88" t="s">
+      <c r="R28" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="S28" s="88" t="s">
+      <c r="S28" s="93" t="s">
         <v>30</v>
       </c>
-      <c r="T28" s="88" t="s">
+      <c r="T28" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="U28" s="88" t="s">
+      <c r="U28" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="V28" s="88" t="s">
+      <c r="V28" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="W28" s="88" t="s">
+      <c r="W28" s="93" t="s">
         <v>86</v>
       </c>
-      <c r="X28" s="90" t="s">
+      <c r="X28" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="Y28" s="92" t="s">
+      <c r="Y28" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="Z28" s="94" t="s">
+      <c r="Z28" s="99" t="s">
         <v>90</v>
       </c>
-      <c r="AA28" s="88" t="s">
+      <c r="AA28" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="AB28" s="88" t="s">
+      <c r="AB28" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="AC28" s="88" t="s">
+      <c r="AC28" s="93" t="s">
         <v>93</v>
       </c>
-      <c r="AD28" s="88" t="s">
+      <c r="AD28" s="93" t="s">
         <v>94</v>
       </c>
-      <c r="AE28" s="88" t="s">
+      <c r="AE28" s="93" t="s">
         <v>95</v>
       </c>
-      <c r="AF28" s="88" t="s">
+      <c r="AF28" s="93" t="s">
         <v>96</v>
       </c>
-      <c r="AG28" s="90" t="s">
+      <c r="AG28" s="95" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:33">
-      <c r="A29" s="93"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="89"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="89"/>
-      <c r="G29" s="89"/>
-      <c r="H29" s="89"/>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="93"/>
-      <c r="M29" s="95"/>
-      <c r="N29" s="89"/>
-      <c r="O29" s="89"/>
-      <c r="P29" s="93"/>
-      <c r="Q29" s="95"/>
-      <c r="R29" s="89"/>
-      <c r="S29" s="89"/>
-      <c r="T29" s="89"/>
-      <c r="U29" s="89"/>
-      <c r="V29" s="89"/>
-      <c r="W29" s="89"/>
-      <c r="X29" s="91"/>
-      <c r="Y29" s="93"/>
-      <c r="Z29" s="95"/>
-      <c r="AA29" s="89"/>
-      <c r="AB29" s="89"/>
-      <c r="AC29" s="89"/>
-      <c r="AD29" s="89"/>
-      <c r="AE29" s="89"/>
-      <c r="AF29" s="89"/>
-      <c r="AG29" s="91"/>
+      <c r="A29" s="98"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="100"/>
+      <c r="D29" s="94"/>
+      <c r="E29" s="94"/>
+      <c r="F29" s="94"/>
+      <c r="G29" s="94"/>
+      <c r="H29" s="94"/>
+      <c r="I29" s="94"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="98"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="94"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="98"/>
+      <c r="Q29" s="100"/>
+      <c r="R29" s="94"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="94"/>
+      <c r="W29" s="94"/>
+      <c r="X29" s="96"/>
+      <c r="Y29" s="98"/>
+      <c r="Z29" s="100"/>
+      <c r="AA29" s="94"/>
+      <c r="AB29" s="94"/>
+      <c r="AC29" s="94"/>
+      <c r="AD29" s="94"/>
+      <c r="AE29" s="94"/>
+      <c r="AF29" s="94"/>
+      <c r="AG29" s="96"/>
     </row>
     <row r="30" spans="1:33">
       <c r="A30" s="52">
@@ -10326,7 +10600,7 @@
         <v>118351994.02845623</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="15.75" thickBot="1">
+    <row r="50" spans="1:33" ht="15" thickBot="1">
       <c r="A50" s="62">
         <v>2011</v>
       </c>
@@ -11782,25 +12056,6 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AD28:AD29"/>
-    <mergeCell ref="AE28:AE29"/>
-    <mergeCell ref="AF28:AF29"/>
-    <mergeCell ref="AG28:AG29"/>
-    <mergeCell ref="Y28:Y29"/>
-    <mergeCell ref="Z28:Z29"/>
-    <mergeCell ref="AA28:AA29"/>
-    <mergeCell ref="AB28:AB29"/>
-    <mergeCell ref="AC28:AC29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
     <mergeCell ref="U28:U29"/>
     <mergeCell ref="V28:V29"/>
     <mergeCell ref="W28:W29"/>
@@ -11815,7 +12070,31 @@
     <mergeCell ref="Q28:Q29"/>
     <mergeCell ref="R28:R29"/>
     <mergeCell ref="S28:S29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="AD28:AD29"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="AF28:AF29"/>
+    <mergeCell ref="AG28:AG29"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="Z28:Z29"/>
+    <mergeCell ref="AA28:AA29"/>
+    <mergeCell ref="AB28:AB29"/>
+    <mergeCell ref="AC28:AC29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated labor data through 2011 for developing countries.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/ChinaDataWorkbook.xlsx
+++ b/data/Excel Workbooks/ChinaDataWorkbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="280" windowWidth="18960" windowHeight="13300" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="280" windowWidth="24620" windowHeight="13300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="China Workbook" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="117">
   <si>
     <t>Exergy [TJ]</t>
   </si>
@@ -876,7 +876,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1170,6 +1170,13 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1743,7 +1750,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="467">
+  <cellStyleXfs count="473">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2217,8 +2224,14 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2474,8 +2487,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="40" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="467">
+  <cellStyles count="473">
     <cellStyle name="•\Ž¦Ï‚Ý‚ÌƒnƒCƒp[ƒŠƒ“ƒN" xfId="42"/>
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 10" xfId="54"/>
@@ -2791,6 +2805,9 @@
     <cellStyle name="Explanatory Text 9" xfId="330"/>
     <cellStyle name="Followed Hyperlink" xfId="464" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="466" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="468" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="470" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="472" builtinId="9" hidden="1"/>
     <cellStyle name="ƒnƒCƒp[ƒŠƒ“ƒN" xfId="44"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Good 10" xfId="331"/>
@@ -2849,6 +2866,9 @@
     <cellStyle name="Heading 4 9" xfId="380"/>
     <cellStyle name="Hyperlink" xfId="463" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="465" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="467" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="469" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="471" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Input 10" xfId="381"/>
     <cellStyle name="Input 11" xfId="382"/>
@@ -3418,16 +3438,16 @@
                   <c:v>1.037689682939687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.050060188644996</c:v>
+                  <c:v>1.050060189449604</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.061531393682739</c:v>
+                  <c:v>1.061531394487346</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.072716259117005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.083751346912529</c:v>
+                  <c:v>1.083751347717136</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1.09440039380697</c:v>
@@ -3463,10 +3483,10 @@
                   <c:v>1.210779484188824</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.21692636170121</c:v>
+                  <c:v>1.216816677641509</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.238102526112724</c:v>
+                  <c:v>1.237991471806884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3813,11 +3833,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2090449480"/>
-        <c:axId val="2090457368"/>
+        <c:axId val="-2121800360"/>
+        <c:axId val="-2121792664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2090449480"/>
+        <c:axId val="-2121800360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3839,6 +3859,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3855,12 +3876,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090457368"/>
+        <c:crossAx val="-2121792664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2090457368"/>
+        <c:axId val="-2121792664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3882,6 +3903,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -3898,7 +3920,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090449480"/>
+        <c:crossAx val="-2121800360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3915,7 +3937,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="91" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -3927,7 +3949,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8669694" cy="6288444"/>
+    <xdr:ext cx="8652747" cy="6280220"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -4696,7 +4718,7 @@
   <dimension ref="A1:BC32"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5049,7 +5071,7 @@
       <c r="B12" s="87">
         <v>574045</v>
       </c>
-      <c r="C12" s="86">
+      <c r="C12" s="101">
         <v>621421200</v>
       </c>
       <c r="D12" s="87">
@@ -5093,7 +5115,7 @@
       <c r="B13" s="87">
         <v>655560</v>
       </c>
-      <c r="C13" s="86">
+      <c r="C13" s="101">
         <v>637471584</v>
       </c>
       <c r="D13" s="87">
@@ -5114,7 +5136,7 @@
         <v>1.1420010626344625</v>
       </c>
       <c r="I13" s="15">
-        <f t="shared" ref="I13:I31" si="3">C13/$C$12</f>
+        <f t="shared" ref="I13:I32" si="3">C13/$C$12</f>
         <v>1.025828510517504</v>
       </c>
       <c r="J13" s="15">
@@ -5137,7 +5159,7 @@
       <c r="B14" s="87">
         <v>747338</v>
       </c>
-      <c r="C14" s="86">
+      <c r="C14" s="101">
         <v>644842368</v>
       </c>
       <c r="D14" s="87">
@@ -5181,8 +5203,8 @@
       <c r="B15" s="87">
         <v>845239</v>
       </c>
-      <c r="C15" s="86">
-        <v>652529662.5</v>
+      <c r="C15" s="101">
+        <v>652529663</v>
       </c>
       <c r="D15" s="87">
         <v>1598493</v>
@@ -5203,7 +5225,7 @@
       </c>
       <c r="I15" s="15">
         <f t="shared" si="3"/>
-        <v>1.0500601886449963</v>
+        <v>1.0500601894496036</v>
       </c>
       <c r="J15" s="15">
         <f t="shared" si="4"/>
@@ -5225,8 +5247,8 @@
       <c r="B16" s="87">
         <v>937370</v>
       </c>
-      <c r="C16" s="86">
-        <v>659658112.5</v>
+      <c r="C16" s="101">
+        <v>659658113</v>
       </c>
       <c r="D16" s="87">
         <v>1797852</v>
@@ -5247,7 +5269,7 @@
       </c>
       <c r="I16" s="15">
         <f t="shared" si="3"/>
-        <v>1.0615313936827389</v>
+        <v>1.0615313944873461</v>
       </c>
       <c r="J16" s="15">
         <f t="shared" si="4"/>
@@ -5269,7 +5291,7 @@
       <c r="B17" s="87">
         <v>1031108</v>
       </c>
-      <c r="C17" s="86">
+      <c r="C17" s="101">
         <v>666608625</v>
       </c>
       <c r="D17" s="87">
@@ -5313,8 +5335,8 @@
       <c r="B18" s="87">
         <v>1127001</v>
       </c>
-      <c r="C18" s="86">
-        <v>673466062.5</v>
+      <c r="C18" s="101">
+        <v>673466063</v>
       </c>
       <c r="D18" s="87">
         <v>2243972</v>
@@ -5335,7 +5357,7 @@
       </c>
       <c r="I18" s="15">
         <f t="shared" si="3"/>
-        <v>1.0837513469125288</v>
+        <v>1.0837513477171361</v>
       </c>
       <c r="J18" s="15">
         <f t="shared" si="4"/>
@@ -5357,7 +5379,7 @@
       <c r="B19" s="87">
         <v>1214907</v>
       </c>
-      <c r="C19" s="86">
+      <c r="C19" s="101">
         <v>680083606</v>
       </c>
       <c r="D19" s="87">
@@ -5401,7 +5423,7 @@
       <c r="B20" s="87">
         <v>1307239</v>
       </c>
-      <c r="C20" s="86">
+      <c r="C20" s="101">
         <v>685997686</v>
       </c>
       <c r="D20" s="87">
@@ -5445,7 +5467,7 @@
       <c r="B21" s="87">
         <v>1417048</v>
       </c>
-      <c r="C21" s="86">
+      <c r="C21" s="101">
         <v>700767975</v>
       </c>
       <c r="D21" s="87">
@@ -5489,7 +5511,7 @@
       <c r="B22" s="87">
         <v>1534663</v>
       </c>
-      <c r="C22" s="86">
+      <c r="C22" s="101">
         <v>696337875</v>
       </c>
       <c r="D22" s="87">
@@ -5533,7 +5555,7 @@
       <c r="B23" s="87">
         <v>1674317</v>
       </c>
-      <c r="C23" s="86">
+      <c r="C23" s="101">
         <v>710365920</v>
       </c>
       <c r="D23" s="87">
@@ -5577,7 +5599,7 @@
       <c r="B24" s="87">
         <v>1841749</v>
       </c>
-      <c r="C24" s="86">
+      <c r="C24" s="101">
         <v>724209640</v>
       </c>
       <c r="D24" s="87">
@@ -5621,7 +5643,7 @@
       <c r="B25" s="87">
         <v>2027765</v>
       </c>
-      <c r="C25" s="86">
+      <c r="C25" s="101">
         <v>718543980</v>
       </c>
       <c r="D25" s="87">
@@ -5665,7 +5687,7 @@
       <c r="B26" s="87">
         <v>2256903</v>
       </c>
-      <c r="C26" s="86">
+      <c r="C26" s="101">
         <v>732169152</v>
       </c>
       <c r="D26" s="87">
@@ -5709,7 +5731,7 @@
       <c r="B27" s="87">
         <v>2543529</v>
       </c>
-      <c r="C27" s="86">
+      <c r="C27" s="101">
         <v>745708176</v>
       </c>
       <c r="D27" s="87">
@@ -5753,7 +5775,7 @@
       <c r="B28" s="87">
         <v>2904710</v>
       </c>
-      <c r="C28" s="86">
+      <c r="C28" s="101">
         <v>749612988</v>
       </c>
       <c r="D28" s="87">
@@ -5797,7 +5819,7 @@
       <c r="B29" s="87">
         <v>3183563</v>
       </c>
-      <c r="C29" s="86">
+      <c r="C29" s="101">
         <v>752404040</v>
       </c>
       <c r="D29" s="87">
@@ -5841,8 +5863,8 @@
       <c r="B30" s="87">
         <v>3476450</v>
       </c>
-      <c r="C30" s="86">
-        <v>756223840</v>
+      <c r="C30" s="101">
+        <v>756155680</v>
       </c>
       <c r="D30" s="87">
         <v>8215729</v>
@@ -5863,7 +5885,7 @@
       </c>
       <c r="I30" s="15">
         <f t="shared" si="3"/>
-        <v>1.21692636170121</v>
+        <v>1.2168166776415095</v>
       </c>
       <c r="J30" s="15">
         <f t="shared" si="4"/>
@@ -5885,8 +5907,8 @@
       <c r="B31" s="87">
         <v>3837181</v>
       </c>
-      <c r="C31" s="86">
-        <v>769383157.5</v>
+      <c r="C31" s="101">
+        <v>769314146</v>
       </c>
       <c r="D31" s="87">
         <v>9288788</v>
@@ -5907,7 +5929,7 @@
       </c>
       <c r="I31" s="15">
         <f t="shared" si="3"/>
-        <v>1.2381025261127236</v>
+        <v>1.2379914718068841</v>
       </c>
       <c r="J31" s="15">
         <f t="shared" si="4"/>
@@ -5929,8 +5951,8 @@
       <c r="B32" s="87">
         <v>4191268</v>
       </c>
-      <c r="C32" s="87" t="s">
-        <v>107</v>
+      <c r="C32" s="101">
+        <v>773009163</v>
       </c>
       <c r="D32" s="87">
         <v>10481215</v>
@@ -5949,8 +5971,9 @@
         <f t="shared" si="2"/>
         <v>7.3012882265327628</v>
       </c>
-      <c r="I32" s="11" t="s">
-        <v>107</v>
+      <c r="I32" s="15">
+        <f t="shared" si="3"/>
+        <v>1.2439375467074505</v>
       </c>
       <c r="J32" s="15">
         <f>D32/$D$12</f>
@@ -5993,7 +6016,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+      <selection sqref="A1:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6160,7 +6183,7 @@
       </c>
       <c r="D5" s="89">
         <f>'China Workbook'!I15</f>
-        <v>1.0500601886449963</v>
+        <v>1.0500601894496036</v>
       </c>
       <c r="E5" s="89">
         <f>'China Workbook'!J15</f>
@@ -6196,7 +6219,7 @@
       </c>
       <c r="D6" s="89">
         <f>'China Workbook'!I16</f>
-        <v>1.0615313936827389</v>
+        <v>1.0615313944873461</v>
       </c>
       <c r="E6" s="89">
         <f>'China Workbook'!J16</f>
@@ -6268,7 +6291,7 @@
       </c>
       <c r="D8" s="89">
         <f>'China Workbook'!I18</f>
-        <v>1.0837513469125288</v>
+        <v>1.0837513477171361</v>
       </c>
       <c r="E8" s="89">
         <f>'China Workbook'!J18</f>
@@ -6700,7 +6723,7 @@
       </c>
       <c r="D20" s="89">
         <f>'China Workbook'!I30</f>
-        <v>1.21692636170121</v>
+        <v>1.2168166776415095</v>
       </c>
       <c r="E20" s="89">
         <f>'China Workbook'!J30</f>
@@ -6736,7 +6759,7 @@
       </c>
       <c r="D21" s="89">
         <f>'China Workbook'!I31</f>
-        <v>1.2381025261127236</v>
+        <v>1.2379914718068841</v>
       </c>
       <c r="E21" s="89">
         <f>'China Workbook'!J31</f>
@@ -6770,9 +6793,9 @@
         <f>'China Workbook'!H32</f>
         <v>7.3012882265327628</v>
       </c>
-      <c r="D22" s="89" t="str">
+      <c r="D22" s="89">
         <f>'China Workbook'!I32</f>
-        <v>NA</v>
+        <v>1.2439375467074505</v>
       </c>
       <c r="E22" s="89">
         <f>'China Workbook'!J32</f>
@@ -6808,7 +6831,7 @@
   <dimension ref="A1:BB41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -12056,6 +12079,25 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="AD28:AD29"/>
+    <mergeCell ref="AE28:AE29"/>
+    <mergeCell ref="AF28:AF29"/>
+    <mergeCell ref="AG28:AG29"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="Z28:Z29"/>
+    <mergeCell ref="AA28:AA29"/>
+    <mergeCell ref="AB28:AB29"/>
+    <mergeCell ref="AC28:AC29"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
     <mergeCell ref="U28:U29"/>
     <mergeCell ref="V28:V29"/>
     <mergeCell ref="W28:W29"/>
@@ -12070,25 +12112,6 @@
     <mergeCell ref="Q28:Q29"/>
     <mergeCell ref="R28:R29"/>
     <mergeCell ref="S28:S29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="AD28:AD29"/>
-    <mergeCell ref="AE28:AE29"/>
-    <mergeCell ref="AF28:AF29"/>
-    <mergeCell ref="AG28:AG29"/>
-    <mergeCell ref="Y28:Y29"/>
-    <mergeCell ref="Z28:Z29"/>
-    <mergeCell ref="AA28:AA29"/>
-    <mergeCell ref="AB28:AB29"/>
-    <mergeCell ref="AC28:AC29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>